<commit_message>
Excel File reader POC
</commit_message>
<xml_diff>
--- a/src/main/resources/samplefile/SampleFile.xlsx
+++ b/src/main/resources/samplefile/SampleFile.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="360" windowWidth="14115" windowHeight="7710"/>
+    <workbookView xWindow="720" yWindow="360" windowWidth="14115" windowHeight="7710" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
+    <sheet name="final" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AA$8</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet2!$A$1:$AA$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet3!$A$1:$AA$1</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="109">
   <si>
     <t>SR. NO.</t>
   </si>
@@ -342,13 +343,19 @@
   </si>
   <si>
     <t>Gender</t>
+  </si>
+  <si>
+    <t>ESIC User</t>
+  </si>
+  <si>
+    <t>ESIC Password</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -376,6 +383,14 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -509,7 +524,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -546,6 +561,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -853,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="U17" sqref="U17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.42578125" defaultRowHeight="15"/>
@@ -1847,4 +1865,131 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AA1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="32.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" s="14" customFormat="1" ht="42" customHeight="1">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y1" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z1" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA1" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>